<commit_message>
Version 1 of the Player Comparison page. Still need to clean up the non-reactive datasets, as well as make the charts more colorful
</commit_message>
<xml_diff>
--- a/Jeopardy Data.xlsx
+++ b/Jeopardy Data.xlsx
@@ -122,6 +122,30 @@
           </rPr>
           <t xml:space="preserve">
 The rat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+*Answered "Year of the Mouse". Later showed that mouse and rat are the same word in Chinese</t>
         </r>
       </text>
     </comment>
@@ -433,12 +457,372 @@
         </r>
       </text>
     </comment>
+    <comment ref="B13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This British author of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">White Teeth, </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">also wrote </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Swing Time</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">, a story of 2 childhood friends who dream of being dancers. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Zadie Smith</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A groundhog named Phil is the center of attention on February 2nd here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Punxsutawney, Pennsylvania</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In 2014 she made history as the first African-American to dance the role Clara in American Ballet theatre's production of </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The Nutcracker. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Misty Copeland</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+*John went back to his desk and came back the next day with the right answer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Beginning in 1867, school was in session for what is now Morehouse College and this university in Washington D.C</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Howard University</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+2013 saw the first congress with 2 African-American Senators when Mo Cowan of Massachusetts served with Tim Scott of this State.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+South Carolina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Two-Hundred pounds of Mulberry leaves fed to worms are used to produce one pound of this fabric</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Silk</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -523,6 +907,18 @@
   <si>
     <t>Economics</t>
   </si>
+  <si>
+    <t>"P"'s on Earth</t>
+  </si>
+  <si>
+    <t>Formulas ar wrong</t>
+  </si>
+  <si>
+    <t>African- American History</t>
+  </si>
+  <si>
+    <t>Fabrics and Textiles</t>
+  </si>
 </sst>
 </file>
 
@@ -531,7 +927,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -614,7 +1010,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -627,11 +1023,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -915,10 +1313,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:AI70"/>
+  <dimension ref="A2:AK70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -957,98 +1355,98 @@
     <col min="35" max="35" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="F2" s="2"/>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <f>SUM(F5:F53)</f>
-        <v>3200</v>
-      </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11">
+        <v>3600</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10">
         <f>SUM(H5:H53)</f>
-        <v>2400</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11">
+        <v>2800</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10">
         <f>SUM(J5:J53)</f>
-        <v>3200</v>
-      </c>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11">
+        <v>3600</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10">
         <f>SUM(L5:L53)</f>
-        <v>5900</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11">
+        <v>9400</v>
+      </c>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10">
         <f>SUM(N5:N53)</f>
-        <v>3200</v>
-      </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11">
+        <v>3600</v>
+      </c>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10">
         <f>SUM(P5:P53)</f>
-        <v>1200</v>
-      </c>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11">
+        <v>3100</v>
+      </c>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10">
         <f>SUM(R5:R53)</f>
         <v>2000</v>
       </c>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11">
+      <c r="T2" s="10"/>
+      <c r="U2" s="10">
         <f>SUM(T5:T53)</f>
-        <v>4100</v>
-      </c>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11">
+        <v>6200</v>
+      </c>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10">
         <f>SUM(V5:V53)</f>
         <v>2800</v>
       </c>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11">
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10">
         <f>SUM(X5:X53)</f>
         <v>1200</v>
       </c>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11">
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10">
         <f>SUM(Z5:Z53)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11">
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10">
         <f>SUM(AB5:AB53)</f>
+        <v>4200</v>
+      </c>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10">
+        <f>SUM(AD5:AD53)</f>
         <v>3800</v>
       </c>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11">
-        <f>SUM(AD5:AD53)</f>
-        <v>3200</v>
-      </c>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="G3">
         <f>SUM(G5:G500)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <f>SUM(I5:I500)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K3">
         <f>SUM(K5:K500)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3">
         <f>SUM(M5:M500)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O3">
         <f>SUM(O5:O500)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q3">
         <f>SUM(Q5:Q500)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S3">
         <f>SUM(S5:S500)</f>
@@ -1056,7 +1454,7 @@
       </c>
       <c r="U3">
         <f>SUM(U5:U500)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="W3">
         <f>SUM(W5:W500)</f>
@@ -1072,16 +1470,16 @@
       </c>
       <c r="AC3">
         <f>SUM(AC5:AC500)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AE3">
         <f>SUM(AE5:AE500)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="6"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1140,12 +1538,12 @@
         <v>22</v>
       </c>
       <c r="AG4" s="6"/>
-      <c r="AH4" s="10" t="s">
+      <c r="AH4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="AI4" s="10"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AI4" s="14"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1262,7 +1660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1368,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="AF6" s="3">
-        <f t="shared" ref="AF6:AF14" si="13">AVERAGE(G6,I6,K6,M6,O6,Q6,S6,U6,W6,Y6,AA6,AC6,AE6)</f>
+        <f t="shared" ref="AF6:AF18" si="13">AVERAGE(G6,I6,K6,M6,O6,Q6,S6,U6,W6,Y6,AA6,AC6,AE6)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AG6" s="6"/>
@@ -1376,12 +1774,12 @@
         <f ca="1">IF(LARGE($G$2:$AE$2,1) = LARGE($G$2:$AE$2,2), "Multiple People", OFFSET($A$4,0,5+MATCH(AI6,$G$2:$AE$2,0)))</f>
         <v>Zach</v>
       </c>
-      <c r="AI6" s="12">
+      <c r="AI6" s="11">
         <f>MAX(G2:AE2)</f>
-        <v>5900</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+        <v>9400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1495,12 +1893,12 @@
         <f ca="1">IF(LARGE($G$2:$AE$2,2) = LARGE($G$2:$AE$2,3), "Multiple People", OFFSET($A$4,0,5+MATCH(AI7,$G$2:$AE$2,0)))</f>
         <v>John</v>
       </c>
-      <c r="AI7" s="12">
+      <c r="AI7" s="11">
         <f>LARGE(G2:AE2,2)</f>
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1614,12 +2012,12 @@
         <f ca="1">IF(LARGE($G$2:$AE$2,3) = LARGE($G$2:$AE$2,4), "Multiple People", OFFSET($A$4,0,5+MATCH(AI8,$G$2:$AE$2,0)))</f>
         <v>Heather</v>
       </c>
-      <c r="AI8" s="12">
+      <c r="AI8" s="11">
         <f ca="1">IF(AH7 = "Multiple People", LARGE(G2:AE2,4),LARGE(G2:AE2,3))</f>
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1733,7 +2131,7 @@
       </c>
       <c r="AG9" s="6"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1850,7 +2248,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1899,6 +2297,9 @@
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
       <c r="P11" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
@@ -1957,7 +2358,7 @@
       </c>
       <c r="AF11" s="3">
         <f t="shared" si="13"/>
-        <v>8.3333333333333329E-2</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="AG11" s="6"/>
       <c r="AH11" s="8" t="str">
@@ -1966,10 +2367,10 @@
       </c>
       <c r="AI11" s="7">
         <f>LARGE($G$3:$AE$3,1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2018,6 +2419,9 @@
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
       <c r="P12" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
@@ -2073,19 +2477,22 @@
       </c>
       <c r="AF12" s="3">
         <f t="shared" si="13"/>
-        <v>0.36363636363636365</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AG12" s="6"/>
       <c r="AH12" s="8" t="str">
         <f ca="1">IF(LARGE($G$3:$AE$3,2) = LARGE($G$3:$AE$3, 3), "Multiple People", OFFSET($A$4,0,5+MATCH(AI12,$G$3:$AE$3,0)))</f>
-        <v>Multiple People</v>
+        <v>John</v>
       </c>
       <c r="AI12" s="7">
         <f>LARGE($G$3:$AE$3,2)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2106,42 +2513,72 @@
         <f t="shared" ref="F13" si="58">IF(G13=1,$E13,"")</f>
         <v/>
       </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
       <c r="H13" s="2" t="str">
         <f t="shared" ref="H13" si="59">IF(I13=1,$E13,"")</f>
         <v/>
       </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
       <c r="J13" s="2" t="str">
         <f t="shared" ref="J13" si="60">IF(K13=1,$E13,"")</f>
         <v/>
       </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
       <c r="L13" s="2" t="str">
         <f t="shared" si="37"/>
         <v/>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="N13" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
       <c r="P13" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
       <c r="R13" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
       <c r="T13" s="2" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
       <c r="V13" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
       <c r="X13" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
       </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
       <c r="Z13" s="2" t="str">
         <f t="shared" si="44"/>
         <v/>
@@ -2150,22 +2587,35 @@
         <f t="shared" si="53"/>
         <v/>
       </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
       <c r="AD13" s="2" t="str">
         <f t="shared" si="54"/>
         <v/>
       </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
       <c r="AH13" s="8" t="str">
-        <f ca="1">IF(LARGE($G$3:$AE$3,3) = LARGE($G$3:$AE$3, 4), "Multiple People", OFFSET($A$4,0,5+MATCH(AI13,$G$3:$AE$3,0)))</f>
-        <v>Matt</v>
+        <f ca="1">IF(AH12="Multiple People",IF(LARGE(G3:AE3,4)=LARGE(G3:AE3,5),"Multiple People",OFFSET(A4,0,5+MATCH(AI13,G3:AE3))),OFFSET(A4,0,5+MATCH(AI13,G3:AE3)))</f>
+        <v>Heather</v>
       </c>
       <c r="AI13" s="7">
-        <f>IF(AI12 = LARGE($G$3:$AE$3,3), LARGE($G$3:$AE$3,4),LARGE($G$3:$AE$3,3))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+        <f>IF(AI12 = LARGE($G$3:$AE$3,3), IF(AI12= LARGE(G3:AE3, 4), LARGE(G3:AE3,5), LARGE($G$3:$AE$3,4)),LARGE($G$3:$AE$3,3))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="1">
         <v>43863</v>
@@ -2181,42 +2631,72 @@
         <f t="shared" ref="F14:F15" si="61">IF(G14=1,$E14,"")</f>
         <v/>
       </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
       <c r="H14" s="2" t="str">
         <f t="shared" ref="H14:H15" si="62">IF(I14=1,$E14,"")</f>
         <v/>
       </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
       <c r="J14" s="2" t="str">
         <f t="shared" ref="J14:J15" si="63">IF(K14=1,$E14,"")</f>
         <v/>
       </c>
-      <c r="L14" s="2" t="str">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
         <f t="shared" si="37"/>
-        <v/>
+        <v>1500</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
       </c>
       <c r="N14" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="P14" s="2" t="str">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
         <f t="shared" si="39"/>
-        <v/>
+        <v>1500</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
       </c>
       <c r="R14" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
-      <c r="T14" s="2" t="str">
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
         <f t="shared" si="41"/>
-        <v/>
+        <v>1500</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
       </c>
       <c r="V14" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
       <c r="X14" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
       </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
       <c r="Z14" s="2" t="str">
         <f t="shared" si="44"/>
         <v/>
@@ -2225,14 +2705,27 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
       <c r="AD14" s="2" t="str">
         <f t="shared" si="46"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="3">
+        <f t="shared" si="13"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
       </c>
       <c r="C15" s="1">
         <v>43864</v>
@@ -2248,42 +2741,72 @@
         <f t="shared" si="61"/>
         <v/>
       </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="62"/>
         <v/>
       </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="63"/>
         <v/>
       </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
       <c r="L15" s="2" t="str">
         <f t="shared" si="37"/>
         <v/>
       </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="N15" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
       <c r="P15" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
       <c r="R15" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
-      <c r="T15" s="2" t="str">
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
         <f t="shared" si="41"/>
-        <v/>
+        <v>200</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
       </c>
       <c r="V15" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
       <c r="X15" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
       </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
       <c r="Z15" s="2" t="str">
         <f t="shared" si="44"/>
         <v/>
@@ -2292,14 +2815,29 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
-      <c r="AD15" s="2" t="str">
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="2">
         <f t="shared" si="46"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15" s="3">
+        <f t="shared" si="13"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="AH15" s="12"/>
+      <c r="AI15" s="12"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="1">
         <v>43865</v>
@@ -2315,38 +2853,65 @@
         <f t="shared" ref="F16" si="64">IF(G16=1,$E16,"")</f>
         <v/>
       </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
       <c r="H16" s="2" t="str">
         <f t="shared" ref="H16" si="65">IF(I16=1,$E16,"")</f>
         <v/>
       </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
       <c r="J16" s="2" t="str">
         <f t="shared" ref="J16" si="66">IF(K16=1,$E16,"")</f>
         <v/>
       </c>
-      <c r="L16" s="2" t="str">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
         <f t="shared" si="37"/>
-        <v/>
+        <v>600</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
       </c>
       <c r="N16" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
       <c r="P16" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
       <c r="R16" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
       <c r="T16" s="2" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
       <c r="V16" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
       <c r="X16" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -2359,14 +2924,29 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
       <c r="AD16" s="2" t="str">
         <f t="shared" si="46"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="3">
+        <f t="shared" si="13"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="AH16" s="13"/>
+      <c r="AI16" s="13"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
       </c>
       <c r="C17" s="1">
         <v>43866</v>
@@ -2382,38 +2962,65 @@
         <f t="shared" ref="F17" si="67">IF(G17=1,$E17,"")</f>
         <v/>
       </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
       <c r="H17" s="2" t="str">
         <f t="shared" ref="H17" si="68">IF(I17=1,$E17,"")</f>
         <v/>
       </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
       <c r="J17" s="2" t="str">
         <f t="shared" ref="J17" si="69">IF(K17=1,$E17,"")</f>
         <v/>
       </c>
-      <c r="L17" s="2" t="str">
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
         <f t="shared" si="37"/>
-        <v/>
+        <v>1000</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
       </c>
       <c r="N17" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
       <c r="P17" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
       <c r="R17" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
       <c r="T17" s="2" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
       <c r="V17" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
       <c r="X17" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -2426,14 +3033,29 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
       <c r="AD17" s="2" t="str">
         <f t="shared" si="46"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="3">
+        <f t="shared" si="13"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="13"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="1">
         <v>43867</v>
@@ -2445,42 +3067,69 @@
       <c r="E18">
         <v>400</v>
       </c>
-      <c r="F18" s="2" t="str">
+      <c r="F18" s="2">
         <f t="shared" ref="F18" si="70">IF(G18=1,$E18,"")</f>
-        <v/>
-      </c>
-      <c r="H18" s="2" t="str">
+        <v>400</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
         <f t="shared" ref="H18" si="71">IF(I18=1,$E18,"")</f>
-        <v/>
-      </c>
-      <c r="J18" s="2" t="str">
+        <v>400</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2">
         <f t="shared" ref="J18" si="72">IF(K18=1,$E18,"")</f>
-        <v/>
-      </c>
-      <c r="L18" s="2" t="str">
+        <v>400</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
         <f t="shared" si="37"/>
-        <v/>
-      </c>
-      <c r="N18" s="2" t="str">
+        <v>400</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="P18" s="2" t="str">
+        <v>400</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18" s="2">
         <f t="shared" si="39"/>
-        <v/>
+        <v>400</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
       </c>
       <c r="R18" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
-      <c r="T18" s="2" t="str">
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
         <f t="shared" si="41"/>
-        <v/>
+        <v>400</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
       </c>
       <c r="V18" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
       <c r="X18" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -2489,18 +3138,33 @@
         <f t="shared" si="44"/>
         <v/>
       </c>
-      <c r="AB18" s="2" t="str">
+      <c r="AB18" s="2">
         <f t="shared" si="45"/>
-        <v/>
-      </c>
-      <c r="AD18" s="2" t="str">
+        <v>400</v>
+      </c>
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="2">
         <f t="shared" si="46"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+      <c r="AE18">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="3">
+        <f t="shared" si="13"/>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="AH18" s="13"/>
+      <c r="AI18" s="13"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="1">
         <v>43868</v>
@@ -2565,9 +3229,12 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
       </c>
       <c r="C20" s="1">
         <v>43869</v>
@@ -2632,7 +3299,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2699,7 +3366,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2766,7 +3433,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
@@ -2833,7 +3500,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -2900,7 +3567,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2967,7 +3634,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3034,7 +3701,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3101,7 +3768,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3168,7 +3835,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -3235,7 +3902,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -3302,7 +3969,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -3369,7 +4036,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5</v>
       </c>
@@ -5987,7 +6654,7 @@
     <mergeCell ref="AH4:AI4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added two add'l pages, created new charts on front page.
</commit_message>
<xml_diff>
--- a/Jeopardy Data.xlsx
+++ b/Jeopardy Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25755" windowHeight="9030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -817,12 +817,396 @@
         </r>
       </text>
     </comment>
+    <comment ref="B19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cotton is a traditional fabric for this activity of making blankets into colorful art</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Quilting</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This shee net fabric with hexagonal holes is named for a french city that began producing it in the early 1800s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tulle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+It's the only capital named for a signer of the Constitution</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Madison, WI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The Mid-1930s TBD Devastator was the first American Naval Aircraft with one of these that could be totally enclosed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cockpit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Members of the Caterpillar Club are those who lives have been saved by using one of these to escape a disabled aircraft</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Parachute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This international airport was named for an agricultural village near London inhabited in Neolithic times</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Heathrow</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Zoe Kazan plays a girlfriend in a coma in this 2017 film co-starring and co-written by Kumail Nanjiani</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The Big Sick</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Never has molding clay been more passionate than when Patrick Swayze and Demi Moore got muddy in this film. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Matthew Jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ghost</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -911,13 +1295,19 @@
     <t>"P"'s on Earth</t>
   </si>
   <si>
-    <t>Formulas ar wrong</t>
-  </si>
-  <si>
     <t>African- American History</t>
   </si>
   <si>
     <t>Fabrics and Textiles</t>
+  </si>
+  <si>
+    <t>State Capitals</t>
+  </si>
+  <si>
+    <t>Aviation</t>
+  </si>
+  <si>
+    <t>Movie Romances</t>
   </si>
 </sst>
 </file>
@@ -973,12 +1363,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1010,7 +1406,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1027,6 +1423,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1313,14 +1711,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:AK70"/>
+  <dimension ref="A2:AI70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
@@ -1331,7 +1730,7 @@
     <col min="10" max="10" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="8" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="15" width="8" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -1339,8 +1738,8 @@
     <col min="18" max="18" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="19" max="19" width="8" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="8" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="5" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="23" max="23" width="8" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="25" max="25" width="8" customWidth="1" collapsed="1"/>
@@ -1355,51 +1754,51 @@
     <col min="35" max="35" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="F2" s="2"/>
       <c r="G2" s="10">
         <f>SUM(F5:F53)</f>
-        <v>3600</v>
+        <v>5600</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10">
         <f>SUM(H5:H53)</f>
-        <v>2800</v>
+        <v>5500</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="10">
         <f>SUM(J5:J53)</f>
-        <v>3600</v>
+        <v>4800</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="10">
         <f>SUM(L5:L53)</f>
-        <v>9400</v>
+        <v>14300</v>
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="10">
         <f>SUM(N5:N53)</f>
-        <v>3600</v>
+        <v>5400</v>
       </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="10">
         <f>SUM(P5:P53)</f>
-        <v>3100</v>
+        <v>6600</v>
       </c>
       <c r="R2" s="10"/>
       <c r="S2" s="10">
         <f>SUM(R5:R53)</f>
-        <v>2000</v>
+        <v>3400</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10">
         <f>SUM(T5:T53)</f>
-        <v>6200</v>
+        <v>10100</v>
       </c>
       <c r="V2" s="10"/>
       <c r="W2" s="10">
         <f>SUM(V5:V53)</f>
-        <v>2800</v>
+        <v>6800</v>
       </c>
       <c r="X2" s="10"/>
       <c r="Y2" s="10">
@@ -1409,56 +1808,56 @@
       <c r="Z2" s="10"/>
       <c r="AA2" s="10">
         <f>SUM(Z5:Z53)</f>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="AB2" s="10"/>
       <c r="AC2" s="10">
         <f>SUM(AB5:AB53)</f>
-        <v>4200</v>
+        <v>9200</v>
       </c>
       <c r="AD2" s="10"/>
       <c r="AE2" s="10">
         <f>SUM(AD5:AD53)</f>
-        <v>3800</v>
+        <v>6000</v>
       </c>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="G3">
         <f>SUM(G5:G500)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I3">
         <f>SUM(I5:I500)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K3">
         <f>SUM(K5:K500)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M3">
         <f>SUM(M5:M500)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="O3">
         <f>SUM(O5:O500)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q3">
         <f>SUM(Q5:Q500)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="S3">
         <f>SUM(S5:S500)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U3">
         <f>SUM(U5:U500)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="W3">
         <f>SUM(W5:W500)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Y3">
         <f>SUM(Y5:Y500)</f>
@@ -1466,20 +1865,20 @@
       </c>
       <c r="AA3">
         <f>SUM(AA5:AA500)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC3">
         <f>SUM(AC5:AC500)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AE3">
         <f>SUM(AE5:AE500)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="6"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1538,12 +1937,12 @@
         <v>22</v>
       </c>
       <c r="AG4" s="6"/>
-      <c r="AH4" s="14" t="s">
+      <c r="AH4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="AI4" s="14"/>
+      <c r="AI4" s="16"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1660,7 +2059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1766,7 +2165,7 @@
         <v>1</v>
       </c>
       <c r="AF6" s="3">
-        <f t="shared" ref="AF6:AF18" si="13">AVERAGE(G6,I6,K6,M6,O6,Q6,S6,U6,W6,Y6,AA6,AC6,AE6)</f>
+        <f t="shared" ref="AF6:AF26" si="13">AVERAGE(G6,I6,K6,M6,O6,Q6,S6,U6,W6,Y6,AA6,AC6,AE6)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AG6" s="6"/>
@@ -1776,10 +2175,10 @@
       </c>
       <c r="AI6" s="11">
         <f>MAX(G2:AE2)</f>
-        <v>9400</v>
+        <v>14300</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1895,10 +2294,10 @@
       </c>
       <c r="AI7" s="11">
         <f>LARGE(G2:AE2,2)</f>
-        <v>6200</v>
+        <v>10100</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2014,10 +2413,10 @@
       </c>
       <c r="AI8" s="11">
         <f ca="1">IF(AH7 = "Multiple People", LARGE(G2:AE2,4),LARGE(G2:AE2,3))</f>
-        <v>4200</v>
+        <v>9200</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2094,7 +2493,7 @@
         <f t="shared" ref="V9:V70" si="42">IF(W9=1,$E9,"")</f>
         <v>600</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="14">
         <v>1</v>
       </c>
       <c r="X9" s="2" t="str">
@@ -2131,7 +2530,7 @@
       </c>
       <c r="AG9" s="6"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2248,7 +2647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2346,7 +2745,7 @@
         <f t="shared" ref="AB11:AB13" si="53">IF(AC11=1,$E11,"")</f>
         <v>400</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="15">
         <v>1</v>
       </c>
       <c r="AD11" s="2" t="str">
@@ -2367,10 +2766,10 @@
       </c>
       <c r="AI11" s="7">
         <f>LARGE($G$3:$AE$3,1)</f>
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2486,13 +2885,10 @@
       </c>
       <c r="AI12" s="7">
         <f>LARGE($G$3:$AE$3,2)</f>
-        <v>7</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2607,10 +3003,10 @@
       </c>
       <c r="AI13" s="7">
         <f>IF(AI12 = LARGE($G$3:$AE$3,3), IF(AI12= LARGE(G3:AE3, 4), LARGE(G3:AE3,5), LARGE($G$3:$AE$3,4)),LARGE($G$3:$AE$3,3))</f>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2720,12 +3116,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1">
         <v>43864</v>
@@ -2832,12 +3228,12 @@
       <c r="AH15" s="12"/>
       <c r="AI15" s="12"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1">
         <v>43865</v>
@@ -2874,7 +3270,7 @@
         <f t="shared" si="37"/>
         <v>600</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="15">
         <v>1</v>
       </c>
       <c r="N16" s="2" t="str">
@@ -2946,7 +3342,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1">
         <v>43866</v>
@@ -2983,7 +3379,7 @@
         <f t="shared" si="37"/>
         <v>1000</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="15">
         <v>1</v>
       </c>
       <c r="N17" s="2" t="str">
@@ -3055,7 +3451,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1">
         <v>43867</v>
@@ -3164,7 +3560,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
         <v>43868</v>
@@ -3176,41 +3572,68 @@
       <c r="E19">
         <v>1200</v>
       </c>
-      <c r="F19" s="2" t="str">
+      <c r="F19" s="2">
         <f t="shared" ref="F19:F20" si="73">IF(G19=1,$E19,"")</f>
-        <v/>
-      </c>
-      <c r="H19" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
         <f t="shared" ref="H19:H20" si="74">IF(I19=1,$E19,"")</f>
-        <v/>
-      </c>
-      <c r="J19" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
         <f t="shared" ref="J19:J20" si="75">IF(K19=1,$E19,"")</f>
-        <v/>
-      </c>
-      <c r="L19" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
         <f t="shared" si="37"/>
-        <v/>
-      </c>
-      <c r="N19" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
         <f t="shared" si="38"/>
-        <v/>
+        <v>1200</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
       </c>
       <c r="P19" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
       <c r="R19" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
       <c r="T19" s="2" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="V19" s="2" t="str">
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19" s="2">
         <f t="shared" si="42"/>
-        <v/>
+        <v>1200</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
       </c>
       <c r="X19" s="2" t="str">
         <f t="shared" si="43"/>
@@ -3220,13 +3643,23 @@
         <f t="shared" si="44"/>
         <v/>
       </c>
-      <c r="AB19" s="2" t="str">
+      <c r="AB19" s="2">
         <f t="shared" si="45"/>
-        <v/>
+        <v>1200</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
       </c>
       <c r="AD19" s="2" t="str">
         <f t="shared" si="46"/>
         <v/>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="3">
+        <f t="shared" si="13"/>
+        <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
@@ -3234,7 +3667,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1">
         <v>43869</v>
@@ -3250,38 +3683,65 @@
         <f t="shared" si="73"/>
         <v/>
       </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
       <c r="H20" s="2" t="str">
         <f t="shared" si="74"/>
         <v/>
       </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="75"/>
         <v/>
       </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
       <c r="L20" s="2" t="str">
         <f t="shared" si="37"/>
         <v/>
       </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="N20" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
       <c r="P20" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
       <c r="R20" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
       <c r="T20" s="2" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
       <c r="V20" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
       <c r="X20" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -3290,19 +3750,32 @@
         <f t="shared" si="44"/>
         <v/>
       </c>
-      <c r="AB20" s="2" t="str">
+      <c r="AB20" s="2">
         <f t="shared" si="45"/>
-        <v/>
+        <v>2000</v>
+      </c>
+      <c r="AC20" s="14">
+        <v>1</v>
       </c>
       <c r="AD20" s="2" t="str">
         <f t="shared" si="46"/>
         <v/>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="3">
+        <f t="shared" si="13"/>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
       <c r="C21" s="1">
         <v>43870</v>
       </c>
@@ -3317,38 +3790,65 @@
         <f t="shared" ref="F21" si="76">IF(G21=1,$E21,"")</f>
         <v/>
       </c>
-      <c r="H21" s="2" t="str">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
         <f t="shared" ref="H21" si="77">IF(I21=1,$E21,"")</f>
-        <v/>
+        <v>1500</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" ref="J21" si="78">IF(K21=1,$E21,"")</f>
         <v/>
       </c>
-      <c r="L21" s="2" t="str">
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
         <f t="shared" si="37"/>
-        <v/>
+        <v>1500</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
       </c>
       <c r="N21" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="P21" s="2" t="str">
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
         <f t="shared" si="39"/>
-        <v/>
+        <v>1500</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
       </c>
       <c r="R21" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
-      <c r="T21" s="2" t="str">
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21" s="2">
         <f t="shared" si="41"/>
-        <v/>
+        <v>1500</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
       </c>
       <c r="V21" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
       <c r="X21" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -3361,15 +3861,28 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
       <c r="AD21" s="2" t="str">
         <f t="shared" si="46"/>
         <v/>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21" s="3">
+        <f t="shared" si="13"/>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
       <c r="C22" s="1">
         <v>43871</v>
       </c>
@@ -3380,42 +3893,69 @@
       <c r="E22">
         <v>200</v>
       </c>
-      <c r="F22" s="2" t="str">
+      <c r="F22" s="2">
         <f t="shared" ref="F22" si="79">IF(G22=1,$E22,"")</f>
-        <v/>
+        <v>200</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
       </c>
       <c r="H22" s="2" t="str">
         <f t="shared" ref="H22" si="80">IF(I22=1,$E22,"")</f>
         <v/>
       </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
       <c r="J22" s="2" t="str">
         <f t="shared" ref="J22" si="81">IF(K22=1,$E22,"")</f>
         <v/>
       </c>
-      <c r="L22" s="2" t="str">
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
         <f t="shared" si="37"/>
-        <v/>
-      </c>
-      <c r="N22" s="2" t="str">
+        <v>200</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22" s="2">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="P22" s="2" t="str">
+        <v>200</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" s="2">
         <f t="shared" si="39"/>
-        <v/>
-      </c>
-      <c r="R22" s="2" t="str">
+        <v>200</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2">
         <f t="shared" si="40"/>
-        <v/>
-      </c>
-      <c r="T22" s="2" t="str">
+        <v>200</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22" s="2">
         <f t="shared" si="41"/>
-        <v/>
+        <v>200</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
       </c>
       <c r="V22" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
       <c r="X22" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -3428,15 +3968,28 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
-      <c r="AD22" s="2" t="str">
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="2">
         <f t="shared" si="46"/>
-        <v/>
+        <v>200</v>
+      </c>
+      <c r="AE22">
+        <v>1</v>
+      </c>
+      <c r="AF22" s="3">
+        <f t="shared" si="13"/>
+        <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4</v>
       </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
       <c r="C23" s="1">
         <v>43872</v>
       </c>
@@ -3447,41 +4000,68 @@
       <c r="E23">
         <v>600</v>
       </c>
-      <c r="F23" s="2" t="str">
+      <c r="F23" s="2">
         <f t="shared" ref="F23" si="82">IF(G23=1,$E23,"")</f>
-        <v/>
+        <v>600</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
       </c>
       <c r="H23" s="2" t="str">
         <f t="shared" ref="H23" si="83">IF(I23=1,$E23,"")</f>
         <v/>
       </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
       <c r="J23" s="2" t="str">
         <f t="shared" ref="J23" si="84">IF(K23=1,$E23,"")</f>
         <v/>
       </c>
-      <c r="L23" s="2" t="str">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
         <f t="shared" si="37"/>
-        <v/>
+        <v>600</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
       </c>
       <c r="N23" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="P23" s="2" t="str">
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2">
         <f t="shared" si="39"/>
-        <v/>
+        <v>600</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
       </c>
       <c r="R23" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
       <c r="T23" s="2" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="V23" s="2" t="str">
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23" s="2">
         <f t="shared" si="42"/>
-        <v/>
+        <v>600</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
       </c>
       <c r="X23" s="2" t="str">
         <f t="shared" si="43"/>
@@ -3491,19 +4071,32 @@
         <f t="shared" si="44"/>
         <v/>
       </c>
-      <c r="AB23" s="2" t="str">
+      <c r="AB23" s="2">
         <f t="shared" si="45"/>
-        <v/>
-      </c>
-      <c r="AD23" s="2" t="str">
+        <v>600</v>
+      </c>
+      <c r="AC23">
+        <v>1</v>
+      </c>
+      <c r="AD23" s="2">
         <f t="shared" si="46"/>
-        <v/>
+        <v>600</v>
+      </c>
+      <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="3">
+        <f t="shared" si="13"/>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
       <c r="C24" s="1">
         <v>43873</v>
       </c>
@@ -3518,37 +4111,64 @@
         <f t="shared" ref="F24:F25" si="85">IF(G24=1,$E24,"")</f>
         <v/>
       </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
       <c r="H24" s="2" t="str">
         <f t="shared" ref="H24:H25" si="86">IF(I24=1,$E24,"")</f>
         <v/>
       </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
       <c r="J24" s="2" t="str">
         <f t="shared" ref="J24:J25" si="87">IF(K24=1,$E24,"")</f>
         <v/>
       </c>
-      <c r="L24" s="2" t="str">
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
         <f t="shared" si="37"/>
-        <v/>
+        <v>1000</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
       </c>
       <c r="N24" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
       <c r="P24" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
       <c r="R24" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
-      <c r="T24" s="2" t="str">
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="V24" s="2" t="str">
+        <v>1000</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24" s="2">
         <f t="shared" si="42"/>
-        <v/>
+        <v>1000</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
       </c>
       <c r="X24" s="2" t="str">
         <f t="shared" si="43"/>
@@ -3562,15 +4182,28 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
-      <c r="AD24" s="2" t="str">
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="2">
         <f t="shared" si="46"/>
-        <v/>
+        <v>1000</v>
+      </c>
+      <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AF24" s="3">
+        <f t="shared" si="13"/>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
       <c r="C25" s="1">
         <v>43874</v>
       </c>
@@ -3585,38 +4218,65 @@
         <f t="shared" si="85"/>
         <v/>
       </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
       <c r="H25" s="2" t="str">
         <f t="shared" si="86"/>
         <v/>
       </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="87"/>
         <v/>
       </c>
-      <c r="L25" s="2" t="str">
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
         <f t="shared" si="37"/>
-        <v/>
-      </c>
-      <c r="N25" s="2" t="str">
+        <v>400</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25" s="2">
         <f t="shared" si="38"/>
-        <v/>
+        <v>400</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
       </c>
       <c r="P25" s="2" t="str">
         <f t="shared" si="39"/>
         <v/>
       </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
       <c r="R25" s="2" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
       <c r="T25" s="2" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
       <c r="V25" s="2" t="str">
         <f t="shared" si="42"/>
         <v/>
       </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
       <c r="X25" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
@@ -3629,15 +4289,28 @@
         <f t="shared" si="45"/>
         <v/>
       </c>
-      <c r="AD25" s="2" t="str">
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="2">
         <f t="shared" si="46"/>
-        <v/>
+        <v>400</v>
+      </c>
+      <c r="AE25">
+        <v>1</v>
+      </c>
+      <c r="AF25" s="3">
+        <f t="shared" si="13"/>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4</v>
       </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
       <c r="C26" s="1">
         <v>43875</v>
       </c>
@@ -3652,58 +4325,98 @@
         <f t="shared" ref="F26" si="88">IF(G26=1,$E26,"")</f>
         <v/>
       </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
       <c r="H26" s="2" t="str">
         <f t="shared" ref="H26" si="89">IF(I26=1,$E26,"")</f>
         <v/>
       </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
       <c r="J26" s="2" t="str">
         <f t="shared" ref="J26" si="90">IF(K26=1,$E26,"")</f>
         <v/>
       </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
       <c r="L26" s="2" t="str">
         <f t="shared" si="37"/>
         <v/>
       </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
       <c r="N26" s="2" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="P26" s="2" t="str">
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
         <f t="shared" si="39"/>
-        <v/>
-      </c>
-      <c r="R26" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26" s="2">
         <f t="shared" si="40"/>
-        <v/>
-      </c>
-      <c r="T26" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26" s="2">
         <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="V26" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26" s="2">
         <f t="shared" si="42"/>
-        <v/>
+        <v>1200</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
       </c>
       <c r="X26" s="2" t="str">
         <f t="shared" si="43"/>
         <v/>
       </c>
-      <c r="Z26" s="2" t="str">
+      <c r="Z26" s="2">
         <f t="shared" si="44"/>
-        <v/>
-      </c>
-      <c r="AB26" s="2" t="str">
+        <v>1200</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="2">
         <f t="shared" si="45"/>
-        <v/>
+        <v>1200</v>
+      </c>
+      <c r="AC26">
+        <v>1</v>
       </c>
       <c r="AD26" s="2" t="str">
         <f t="shared" si="46"/>
         <v/>
+      </c>
+      <c r="AF26" s="3">
+        <f t="shared" si="13"/>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
       </c>
       <c r="C27" s="1">
         <v>43876</v>

</xml_diff>